<commit_message>
Fixed equation for 10k resistor
</commit_message>
<xml_diff>
--- a/Hypnos V3.2/Bill of Materials - Hypnos V3.2.xlsx
+++ b/Hypnos V3.2/Bill of Materials - Hypnos V3.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tek\Desktop\Store\Hypnos V3.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namig\Desktop\Hypnos\Hypnos V3\3.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A48CFEA-4FE3-4F6A-BB4A-911452A06413}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38617F51-BE34-41AB-8DBC-757904BE8041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -693,23 +695,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1"/>
-    <col min="4" max="4" width="31.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.81640625" style="1"/>
+    <col min="2" max="2" width="27.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" style="1"/>
+    <col min="4" max="4" width="31.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -738,7 +740,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -770,7 +772,7 @@
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -802,7 +804,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -834,7 +836,7 @@
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -851,7 +853,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -883,7 +885,7 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
@@ -915,7 +917,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -945,7 +947,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -975,7 +977,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -990,7 +992,7 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1024,7 @@
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1054,7 @@
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>0</v>
       </c>
@@ -1068,8 +1070,9 @@
       <c r="E13" s="14">
         <v>0.1</v>
       </c>
-      <c r="F13" s="14">
-        <v>0.1</v>
+      <c r="F13" s="12">
+        <f>E13*C13</f>
+        <v>0.2</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>61</v>
@@ -1083,7 +1086,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1118,7 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1150,7 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>0</v>
       </c>
@@ -1179,7 +1182,7 @@
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
@@ -1211,7 +1214,7 @@
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>0</v>
       </c>
@@ -1243,7 +1246,7 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>0</v>
       </c>
@@ -1273,7 +1276,7 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1283,7 +1286,7 @@
       </c>
       <c r="F20" s="9">
         <f>SUM(F2:F19)</f>
-        <v>16.46</v>
+        <v>16.559999999999999</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
@@ -1293,7 +1296,7 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1308,7 +1311,7 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1321,7 +1324,7 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1336,7 +1339,7 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1381,22 +1384,22 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="9"/>
-    <col min="7" max="7" width="20.5703125" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="7.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.26953125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="9"/>
+    <col min="7" max="7" width="20.54296875" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1419,7 +1422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>30</v>
       </c>
@@ -1473,7 +1476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1503,12 +1506,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="D5" s="2"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1562,7 +1565,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>30</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -1615,13 +1618,13 @@
       </c>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="D10" s="2"/>
       <c r="F10" s="14"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>30</v>
       </c>
@@ -1651,7 +1654,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1676,7 +1679,7 @@
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
@@ -1703,7 +1706,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
@@ -1730,7 +1733,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>30</v>
       </c>
@@ -1784,7 +1787,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>30</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>0</v>
       </c>
@@ -1866,7 +1869,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E20" s="9" t="s">
         <v>5</v>
       </c>
@@ -1902,23 +1905,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00EFBA5-BB63-4E95-AAB6-77207EAA5FF2}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="9" customWidth="1"/>
     <col min="2" max="2" width="24" style="9" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="9"/>
-    <col min="4" max="4" width="24.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="9"/>
-    <col min="7" max="7" width="19.140625" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="9"/>
+    <col min="3" max="3" width="9.1796875" style="9"/>
+    <col min="4" max="4" width="24.453125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="9"/>
+    <col min="7" max="7" width="19.1796875" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -1995,7 +1998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
@@ -2022,12 +2025,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="D5" s="2"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>38</v>
       </c>
@@ -2054,7 +2057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -2106,7 +2109,7 @@
       </c>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
@@ -2131,12 +2134,12 @@
       </c>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="D10" s="2"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
@@ -2163,7 +2166,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
@@ -2188,7 +2191,7 @@
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
@@ -2242,7 +2245,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -2269,7 +2272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>38</v>
       </c>
@@ -2296,7 +2299,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>38</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>38</v>
       </c>
@@ -2350,7 +2353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>38</v>
       </c>
@@ -2378,7 +2381,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E20" s="9" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Updated documentation (BOM, components in schematics, pick-n-place file)
</commit_message>
<xml_diff>
--- a/Hypnos V3.2/Bill of Materials - Hypnos V3.2.xlsx
+++ b/Hypnos V3.2/Bill of Materials - Hypnos V3.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namig\Desktop\Hypnos\Hypnos V3\3.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namig\Documents\GitHub\OPEnS-Hypnos\Hypnos V3.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38617F51-BE34-41AB-8DBC-757904BE8041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E3F53D-FD33-45EA-ACA5-F2C2FA4CF254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="78">
   <si>
     <t>Digikey</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>100pF Capacitor</t>
-  </si>
-  <si>
-    <t>399-1122-1-ND</t>
   </si>
   <si>
     <t>P channel Mosfet - Large</t>
@@ -693,25 +690,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1"/>
-    <col min="2" max="2" width="27.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" style="1"/>
-    <col min="4" max="4" width="31.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="31.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -740,7 +737,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -761,7 +758,7 @@
         <v>0.66</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -772,12 +769,12 @@
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -793,7 +790,7 @@
         <v>0.41</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -804,7 +801,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -825,18 +822,18 @@
         <v>0.34</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -853,7 +850,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -864,7 +861,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="9">
         <v>0.1</v>
@@ -874,7 +871,7 @@
         <v>0.2</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -885,7 +882,7 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
@@ -906,7 +903,7 @@
         <v>0.2</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -917,7 +914,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -938,7 +935,7 @@
         <v>1.95</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -947,7 +944,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -968,7 +965,7 @@
         <v>8.77</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -977,7 +974,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -992,7 +989,7 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1010,7 @@
         <v>0.68</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -1024,7 +1021,7 @@
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1042,7 @@
         <v>0.91</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -1054,7 +1051,7 @@
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>0</v>
       </c>
@@ -1075,7 +1072,7 @@
         <v>0.2</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1086,7 +1083,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1104,7 @@
         <v>0.38</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -1118,7 +1115,7 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1136,7 @@
         <v>1.02</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -1150,18 +1147,18 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" s="9">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="E16" s="9">
         <v>0.1</v>
@@ -1171,7 +1168,7 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -1182,18 +1179,18 @@
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C17" s="9">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="E17" s="9">
         <v>0.1</v>
@@ -1203,7 +1200,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -1214,108 +1211,91 @@
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C18" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E18" s="9">
-        <v>0.1</v>
+        <v>0.44</v>
       </c>
       <c r="F18" s="9">
         <f>E18*C18</f>
-        <v>0.2</v>
+        <v>0.44</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="K18" s="10"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="9">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0.44</v>
+    <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F19" s="9">
-        <f>E19*C19</f>
-        <v>0.44</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>61</v>
-      </c>
+        <f>SUM(F2:F18)</f>
+        <v>16.36</v>
+      </c>
+      <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
-      <c r="K19" s="10"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="9">
-        <f>SUM(F2:F19)</f>
-        <v>16.559999999999999</v>
-      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="11"/>
+      <c r="K20" s="10"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="D21" s="2"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="10"/>
+      <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="2"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -1324,11 +1304,11 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -1338,21 +1318,6 @@
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-    </row>
-    <row r="24" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1371,11 +1336,10 @@
     <hyperlink ref="A15" r:id="rId12" xr:uid="{247168BD-CAA9-4A4B-895A-7D9DDE2FA1DF}"/>
     <hyperlink ref="A16" r:id="rId13" xr:uid="{D8A6FD20-2450-48AF-83CD-A30DFDFC1640}"/>
     <hyperlink ref="A17" r:id="rId14" xr:uid="{F0E6A2CD-5756-47EA-97FE-47F340C712F7}"/>
-    <hyperlink ref="A18" r:id="rId15" xr:uid="{59CB5D16-F71B-411F-96E1-F6283CA24023}"/>
-    <hyperlink ref="A19" r:id="rId16" xr:uid="{86C968D4-D1F1-48D3-BEA1-BEAA5BFA5545}"/>
+    <hyperlink ref="A18" r:id="rId15" xr:uid="{86C968D4-D1F1-48D3-BEA1-BEAA5BFA5545}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -1387,19 +1351,19 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.26953125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="9"/>
-    <col min="7" max="7" width="20.54296875" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="9"/>
+    <col min="1" max="1" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="9"/>
+    <col min="7" max="7" width="20.5703125" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1422,7 +1386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
@@ -1433,7 +1397,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="9">
         <v>0.15</v>
@@ -1443,13 +1407,13 @@
         <v>0.15</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>30</v>
       </c>
@@ -1470,18 +1434,18 @@
         <v>0.62</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -1497,21 +1461,21 @@
         <v>0.41</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="D5" s="2"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
@@ -1522,7 +1486,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="9">
         <v>0.1</v>
@@ -1532,13 +1496,13 @@
         <v>0.2</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1559,13 +1523,13 @@
         <v>0.2</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K7" s="13">
         <v>1206</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>30</v>
       </c>
@@ -1586,14 +1550,14 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -1614,17 +1578,17 @@
         <v>8.77</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="D10" s="2"/>
       <c r="F10" s="14"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>30</v>
       </c>
@@ -1645,7 +1609,7 @@
         <v>0.66</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>24</v>
@@ -1654,7 +1618,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1675,11 +1639,11 @@
         <v>0.91</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
@@ -1700,13 +1664,13 @@
         <v>0.18</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K13" s="13">
         <v>1206</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
@@ -1727,13 +1691,13 @@
         <v>0.36</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K14" s="13">
         <v>1206</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -1754,24 +1718,24 @@
         <v>0.86</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="9">
         <v>0.1</v>
@@ -1781,24 +1745,24 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E17" s="9">
         <v>0.1</v>
@@ -1808,13 +1772,13 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>30</v>
       </c>
@@ -1825,7 +1789,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="9">
         <v>0.1</v>
@@ -1835,24 +1799,24 @@
         <v>0.2</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K18" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C19" s="9">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E19" s="9">
         <v>0.44</v>
@@ -1862,14 +1826,14 @@
         <v>0.44</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E20" s="9" t="s">
         <v>5</v>
       </c>
@@ -1909,19 +1873,19 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="9" customWidth="1"/>
     <col min="2" max="2" width="24" style="9" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="9"/>
-    <col min="4" max="4" width="24.453125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="9"/>
-    <col min="7" max="7" width="19.1796875" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="9"/>
+    <col min="3" max="3" width="9.140625" style="9"/>
+    <col min="4" max="4" width="24.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="9"/>
+    <col min="7" max="7" width="19.140625" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1944,7 +1908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
@@ -1955,7 +1919,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="9">
         <v>0.16</v>
@@ -1965,13 +1929,13 @@
         <v>0.32</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -1992,24 +1956,24 @@
         <v>0.66</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="9">
         <v>0.39</v>
@@ -2019,18 +1983,18 @@
         <v>0.39</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="D5" s="2"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>38</v>
       </c>
@@ -2041,7 +2005,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="9">
         <v>0.1</v>
@@ -2051,13 +2015,13 @@
         <v>0.2</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
@@ -2068,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="9">
         <v>0.1</v>
@@ -2078,13 +2042,13 @@
         <v>0.2</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7" s="13">
         <v>1206</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -2105,11 +2069,11 @@
         <v>1.95</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
@@ -2130,16 +2094,16 @@
         <v>9.0399999999999991</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="D10" s="2"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
@@ -2160,13 +2124,13 @@
         <v>0.68</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
@@ -2187,11 +2151,11 @@
         <v>0.91</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
@@ -2202,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" s="14">
         <v>0.15</v>
@@ -2212,13 +2176,13 @@
         <v>0.3</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K13" s="13">
         <v>1206</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
@@ -2239,13 +2203,13 @@
         <v>0.52</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K14" s="13">
         <v>1206</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -2266,24 +2230,24 @@
         <v>1</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="9">
         <v>0.1</v>
@@ -2293,24 +2257,24 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="9">
         <v>0.23</v>
@@ -2320,13 +2284,13 @@
         <v>0.23</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>38</v>
       </c>
@@ -2337,7 +2301,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="9">
         <v>0.1</v>
@@ -2347,24 +2311,24 @@
         <v>0.2</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K18" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="9">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="9">
         <v>0.44</v>
@@ -2374,14 +2338,14 @@
         <v>0.44</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E20" s="9" t="s">
         <v>5</v>
       </c>

</xml_diff>